<commit_message>
Added Dead volume, adjusted few lables, added option to print all components in result page compare experimental data
</commit_message>
<xml_diff>
--- a/docu/LossFunctionExperimentSet/TestExperiment3.xlsx
+++ b/docu/LossFunctionExperimentSet/TestExperiment3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA8C6F1-A8F8-466E-938A-A093BE7FB3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F340EB5E-825C-468F-BEFC-2F53F3E0636C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="2205" windowWidth="17070" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="125">
   <si>
     <t>Experiment conditions</t>
   </si>
@@ -392,6 +392,9 @@
   </si>
   <si>
     <t>0,0499</t>
+  </si>
+  <si>
+    <t>deadVolume</t>
   </si>
 </sst>
 </file>
@@ -751,9 +754,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -772,7 +774,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -815,6 +816,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -1095,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,744 +1110,752 @@
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="23">
         <v>235</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="23">
         <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="23">
         <v>150</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="22">
         <v>44496</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="23">
         <v>0.85</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>0</v>
-      </c>
-      <c r="B10" s="16">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+    <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>0</v>
+      </c>
+      <c r="B10" s="14">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>2</v>
       </c>
-      <c r="B11" s="16">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="B11" s="14">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
         <v>4</v>
       </c>
-      <c r="B12" s="16">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="17" t="s">
+      <c r="B12" s="14">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+    <row r="13" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
         <v>6</v>
       </c>
-      <c r="B13" s="16">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="17" t="s">
+      <c r="B13" s="14">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
+    <row r="14" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
         <v>8</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="4">
-        <v>0</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="17" t="s">
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+    <row r="15" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
         <v>10</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="4">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="17" t="s">
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+    <row r="16" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
         <v>12</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="17" t="s">
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="4">
-        <v>0</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
-      <c r="E17" s="18">
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="16">
         <v>1.1222000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="4">
-        <v>0</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="18">
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="16">
         <v>1.3787</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="4">
-        <v>0</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="18">
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="16">
         <v>1.5543</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>20</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="4">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="18">
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="16">
         <v>1.5542</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
+      <c r="A21" s="5">
         <v>22</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="4">
-        <v>0</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
-      <c r="E21" s="18">
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="16">
         <v>1.4292</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6">
+      <c r="A22" s="5">
         <v>24</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="4">
-        <v>0</v>
-      </c>
-      <c r="E22" s="18">
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="16">
         <v>1.2626999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6">
+      <c r="A23" s="5">
         <v>26</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="4">
-        <v>0</v>
-      </c>
-      <c r="E23" s="18">
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="16">
         <v>1.0003</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6">
+      <c r="A24" s="5">
         <v>28</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6">
+      <c r="A25" s="5">
         <v>30</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6">
+      <c r="A26" s="5">
         <v>32</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="15" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6">
+      <c r="A27" s="5">
         <v>34</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="15" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6">
+      <c r="A28" s="5">
         <v>36</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6">
+      <c r="A29" s="5">
         <v>38</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6">
+      <c r="A30" s="5">
         <v>40</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6">
+      <c r="A31" s="5">
         <v>45</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="6">
+      <c r="A32" s="5">
         <v>50</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="15" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6">
+      <c r="A33" s="5">
         <v>55</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E33" s="15" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6">
+      <c r="A34" s="5">
         <v>60</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E34" s="15" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6">
+      <c r="A35" s="5">
         <v>65</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="15" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6">
+      <c r="A36" s="5">
         <v>70</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="15" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6">
+      <c r="A37" s="5">
         <v>75</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="15" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6">
+      <c r="A38" s="5">
         <v>80</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6">
+      <c r="A39" s="5">
         <v>85</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="15" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="6">
+      <c r="A40" s="5">
         <v>90</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6">
+      <c r="A41" s="5">
         <v>105</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E41" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="6">
+      <c r="A42" s="5">
         <v>120</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="E42" s="15" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="6">
+      <c r="A43" s="5">
         <v>135</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E43" s="15" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="6">
+      <c r="A44" s="5">
         <v>150</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="E44" s="15" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="6">
+      <c r="A45" s="5">
         <v>165</v>
       </c>
-      <c r="B45" s="16">
-        <v>0</v>
-      </c>
-      <c r="C45" s="4" t="s">
+      <c r="B45" s="14">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E45" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7">
+      <c r="A46" s="6">
         <v>180</v>
       </c>
-      <c r="B46" s="19">
-        <v>0</v>
-      </c>
-      <c r="C46" s="20">
-        <v>0</v>
-      </c>
-      <c r="D46" s="20" t="s">
+      <c r="B46" s="17">
+        <v>0</v>
+      </c>
+      <c r="C46" s="18">
+        <v>0</v>
+      </c>
+      <c r="D46" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="19" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>